<commit_message>
Versão Testes 1.0 Instalado no timer em uso.
</commit_message>
<xml_diff>
--- a/Timer/Valor_custo_timer.xlsx
+++ b/Timer/Valor_custo_timer.xlsx
@@ -89,7 +89,7 @@
     <t>Caixa</t>
   </si>
   <si>
-    <t>Conectores</t>
+    <t>Conectores h</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(D:D)</f>
-        <v>173.05999999999997</v>
+        <v>210.46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,11 +522,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D15" si="0">B5*C5</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -558,11 +558,11 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -576,11 +576,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>5.9</v>
+        <v>7.8</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>5.9</v>
+        <v>7.8</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -684,11 +684,11 @@
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -702,11 +702,11 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>